<commit_message>
Actualizo diario y excel
</commit_message>
<xml_diff>
--- a/lista.xlsx
+++ b/lista.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\OneDrive\Escritorio\Máster\TFM\Listado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\TFM-Maria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29135110-6FE7-4DA8-94AE-7D7F51DD7E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F4FFF2-BB89-444C-BCB0-FD9D9E7F7DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="164">
   <si>
     <t>Nº</t>
   </si>
@@ -520,6 +521,15 @@
   </si>
   <si>
     <t>HD 36408A y B: es un sist binario?? En sector 6 incluye 2 estrellas dentro de la apertura (en .dat solo aparece una), en los demás sectores no incluye ninguna estrella dentro de la apertura (solo el sector 44 tiene una estrella dentro de la apertura en .dat)</t>
+  </si>
+  <si>
+    <t>P teórico</t>
+  </si>
+  <si>
+    <t>P obtenido</t>
+  </si>
+  <si>
+    <t>COMBINED</t>
   </si>
 </sst>
 </file>
@@ -554,7 +564,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,6 +610,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -778,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -861,65 +883,125 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1209,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2517,20 +2599,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{039A85D4-5E63-47A8-9899-65C28110F43B}">
-  <dimension ref="A1:F111"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView topLeftCell="A95" workbookViewId="0">
+      <selection sqref="A1:H111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16.77734375" customWidth="1"/>
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="45" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -2546,18 +2629,24 @@
       <c r="E1" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" s="26" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="34">
+      <c r="C2" s="45">
         <v>75311623</v>
       </c>
       <c r="D2" s="18">
@@ -2566,33 +2655,39 @@
       <c r="E2" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="F2" s="38"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="44"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="19">
         <v>8</v>
       </c>
       <c r="E3" s="21">
         <v>1310.8510000000001</v>
       </c>
-      <c r="F3" s="36"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="39"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="22">
         <v>9</v>
       </c>
       <c r="E4" s="23">
         <v>1310.8510000000001</v>
       </c>
-      <c r="F4" s="37"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" s="54"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="40"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>12</v>
       </c>
@@ -2602,697 +2697,801 @@
       <c r="C5" s="29">
         <v>49720925</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="30">
         <v>18</v>
       </c>
       <c r="E5" s="19">
         <v>0</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="56"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="19" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="47">
         <v>435781776</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="30">
         <v>14</v>
       </c>
       <c r="E6" s="19">
         <v>1.296</v>
       </c>
-      <c r="F6" s="35"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="49">
+      <c r="F6" s="56"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="38"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="31">
         <v>41</v>
       </c>
       <c r="E7" s="19">
         <v>1.232</v>
       </c>
-      <c r="F7" s="36"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="49">
+      <c r="F7" s="56"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="39"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="31">
         <v>54</v>
       </c>
       <c r="E8" s="19">
         <v>1.8460000000000001</v>
       </c>
-      <c r="F8" s="36"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="49">
+      <c r="F8" s="56"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="39"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="31">
         <v>81</v>
       </c>
       <c r="E9" s="19">
         <v>2.7269999999999999</v>
       </c>
-      <c r="F9" s="37"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
+      <c r="F9" s="56"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="40"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="48">
         <v>434408053</v>
       </c>
-      <c r="D10" s="49">
+      <c r="D10" s="31">
         <v>1</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="57"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="38" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="49">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="48"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="31">
         <v>2</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="F11" s="36"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="48">
+      <c r="F11" s="57"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="39"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="48"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="30">
         <v>6</v>
       </c>
       <c r="E12" s="19">
         <v>0</v>
       </c>
-      <c r="F12" s="36"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="49">
+      <c r="F12" s="56"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="39"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="48"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="31">
         <v>33</v>
       </c>
       <c r="E13" s="19">
         <v>0</v>
       </c>
-      <c r="F13" s="36"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="49">
+      <c r="F13" s="56"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="39"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="48"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="31">
         <v>43</v>
       </c>
       <c r="E14" s="19">
         <v>0</v>
       </c>
-      <c r="F14" s="36"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="49">
+      <c r="F14" s="56"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="39"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="48"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="31">
         <v>44</v>
       </c>
       <c r="E15" s="19">
         <v>0</v>
       </c>
-      <c r="F15" s="36"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="49">
+      <c r="F15" s="56"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="39"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="48"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="31">
         <v>45</v>
       </c>
       <c r="E16" s="19">
         <v>0</v>
       </c>
-      <c r="F16" s="36"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="49">
+      <c r="F16" s="56"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="39"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="48"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="31">
         <v>71</v>
       </c>
       <c r="E17" s="19">
         <v>0</v>
       </c>
-      <c r="F17" s="36"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="49">
+      <c r="F17" s="56"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="39"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="48"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="31">
         <v>72</v>
       </c>
       <c r="E18" s="19">
         <v>0</v>
       </c>
-      <c r="F18" s="36"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="49">
+      <c r="F18" s="56"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="39"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="48"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="31">
         <v>87</v>
       </c>
       <c r="E19" s="19">
         <v>0</v>
       </c>
-      <c r="F19" s="37"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="31" t="s">
+      <c r="F19" s="56"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="40"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="31">
+      <c r="C20" s="48">
         <v>329074395</v>
       </c>
-      <c r="D20" s="48">
+      <c r="D20" s="30">
         <v>15</v>
       </c>
       <c r="E20" s="19">
         <v>0</v>
       </c>
-      <c r="F20" s="39" t="s">
+      <c r="F20" s="56"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="32" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="49">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="48"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="31">
         <v>16</v>
       </c>
       <c r="E21" s="19">
         <v>1.3280000000000001</v>
       </c>
-      <c r="F21" s="40"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="49">
+      <c r="F21" s="56"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="33"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="48"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="31">
         <v>17</v>
       </c>
       <c r="E22" s="19">
         <v>1.3280000000000001</v>
       </c>
-      <c r="F22" s="40"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="49">
+      <c r="F22" s="56"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="33"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="48"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="31">
         <v>84</v>
       </c>
       <c r="E23" s="19">
         <v>0</v>
       </c>
-      <c r="F23" s="41"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="31" t="s">
+      <c r="F23" s="56"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="34"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="31">
+      <c r="C24" s="48">
         <v>316493106</v>
       </c>
-      <c r="D24" s="48">
+      <c r="D24" s="30">
         <v>24</v>
       </c>
       <c r="E24" s="19">
         <v>0</v>
       </c>
-      <c r="F24" s="35" t="s">
+      <c r="F24" s="56"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="38" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="49">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="48"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="31">
         <v>25</v>
       </c>
       <c r="E25" s="19"/>
-      <c r="F25" s="36"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="49">
+      <c r="F25" s="56"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="39"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="48"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="31">
         <v>26</v>
       </c>
       <c r="E26" s="19"/>
-      <c r="F26" s="37"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="32" t="s">
+      <c r="F26" s="56"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="40"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="47">
         <v>304996702</v>
       </c>
-      <c r="D27" s="48">
+      <c r="D27" s="30">
         <v>10</v>
       </c>
       <c r="E27" s="19">
         <v>0.47099999999999997</v>
       </c>
-      <c r="F27" s="35"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="32"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="49">
+      <c r="F27" s="56"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="38"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="47"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="31">
         <v>11</v>
       </c>
       <c r="E28" s="19">
         <v>1.024</v>
       </c>
-      <c r="F28" s="36"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="32"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="49">
+      <c r="F28" s="56"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="39"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="47"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="31">
         <v>90</v>
       </c>
       <c r="E29" s="19">
         <v>0.47099999999999997</v>
       </c>
-      <c r="F29" s="37"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="31" t="s">
+      <c r="F29" s="56"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="40"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="31">
+      <c r="C30" s="48">
         <v>302824830</v>
       </c>
-      <c r="D30" s="48">
+      <c r="D30" s="30">
         <v>6</v>
       </c>
       <c r="E30" s="19">
         <v>0</v>
       </c>
-      <c r="F30" s="42" t="s">
+      <c r="F30" s="56"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="35" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="49">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="48"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="31">
         <v>43</v>
       </c>
       <c r="E31" s="19">
         <v>0</v>
       </c>
-      <c r="F31" s="43"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="49">
+      <c r="F31" s="56"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="36"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="48"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="31">
         <v>44</v>
       </c>
       <c r="E32" s="19">
         <v>0</v>
       </c>
-      <c r="F32" s="43"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="49">
+      <c r="F32" s="56"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="36"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="48"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="31">
         <v>45</v>
       </c>
       <c r="E33" s="19">
         <v>0</v>
       </c>
-      <c r="F33" s="43"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="49">
+      <c r="F33" s="56"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="36"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="48"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="31">
         <v>71</v>
       </c>
       <c r="E34" s="19">
         <v>0</v>
       </c>
-      <c r="F34" s="44"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="32" t="s">
+      <c r="F34" s="56"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="37"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="32">
+      <c r="C35" s="47">
         <v>284141111</v>
       </c>
-      <c r="D35" s="49">
+      <c r="D35" s="31">
         <v>17</v>
       </c>
       <c r="E35" s="19">
         <v>1.069</v>
       </c>
-      <c r="F35" s="35"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="32"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="48">
+      <c r="F35" s="56"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="38"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="47"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="30">
         <v>18</v>
       </c>
       <c r="E36" s="19">
         <v>1.6859999999999999</v>
       </c>
-      <c r="F36" s="36"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="32"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="49">
+      <c r="F36" s="56"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="39"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="47"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="31">
         <v>85</v>
       </c>
       <c r="E37" s="19">
         <v>1.6859999999999999</v>
       </c>
-      <c r="F37" s="37"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="31" t="s">
+      <c r="F37" s="56"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="40"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="31">
+      <c r="C38" s="48">
         <v>277502552</v>
       </c>
-      <c r="D38" s="49">
+      <c r="D38" s="31">
         <v>14</v>
       </c>
       <c r="E38" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="F38" s="42" t="s">
+      <c r="F38" s="57"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="35" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="49">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="48"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="31">
         <v>15</v>
       </c>
       <c r="E39" s="19">
         <v>0</v>
       </c>
-      <c r="F39" s="43"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="31"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="48">
+      <c r="F39" s="56"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="36"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="48"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="30">
         <v>16</v>
       </c>
       <c r="E40" s="19">
         <v>0</v>
       </c>
-      <c r="F40" s="43"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="31"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="49">
+      <c r="F40" s="56"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="36"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="48"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="31">
         <v>17</v>
       </c>
       <c r="E41" s="19">
         <v>0</v>
       </c>
-      <c r="F41" s="43"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="31"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="49">
+      <c r="F41" s="56"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="36"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="48"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="31">
         <v>55</v>
       </c>
       <c r="E42" s="19">
         <v>0</v>
       </c>
-      <c r="F42" s="43"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="31"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="49">
+      <c r="F42" s="56"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="36"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="48"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="31">
         <v>56</v>
       </c>
       <c r="E43" s="19">
         <v>0</v>
       </c>
-      <c r="F43" s="43"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="31"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="49">
+      <c r="F43" s="56"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="36"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="48"/>
+      <c r="B44" s="48"/>
+      <c r="C44" s="48"/>
+      <c r="D44" s="31">
         <v>57</v>
       </c>
       <c r="E44" s="19">
         <v>0</v>
       </c>
-      <c r="F44" s="43"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="31"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="49">
+      <c r="F44" s="56"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="36"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="48"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="31">
         <v>75</v>
       </c>
       <c r="E45" s="19">
         <v>0</v>
       </c>
-      <c r="F45" s="43"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="31"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="49">
+      <c r="F45" s="56"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="36"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="48"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="31">
         <v>76</v>
       </c>
       <c r="E46" s="19">
         <v>0</v>
       </c>
-      <c r="F46" s="43"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="31"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="49">
+      <c r="F46" s="56"/>
+      <c r="G46" s="52"/>
+      <c r="H46" s="36"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="48"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="31">
         <v>77</v>
       </c>
       <c r="E47" s="19">
         <v>0</v>
       </c>
-      <c r="F47" s="43"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="31"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="49">
+      <c r="F47" s="56"/>
+      <c r="G47" s="52"/>
+      <c r="H47" s="36"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="48"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="31">
         <v>82</v>
       </c>
       <c r="E48" s="19">
         <v>0</v>
       </c>
-      <c r="F48" s="43"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="31"/>
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="49">
+      <c r="F48" s="56"/>
+      <c r="G48" s="52"/>
+      <c r="H48" s="36"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="48"/>
+      <c r="B49" s="48"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="31">
         <v>84</v>
       </c>
       <c r="E49" s="19">
         <v>0</v>
       </c>
-      <c r="F49" s="44"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="31" t="s">
+      <c r="F49" s="56"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="37"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="31">
+      <c r="C50" s="48">
         <v>310883625</v>
       </c>
-      <c r="D50" s="48">
+      <c r="D50" s="30">
         <v>11</v>
       </c>
       <c r="E50" s="19">
         <v>0</v>
       </c>
-      <c r="F50" s="42" t="s">
+      <c r="F50" s="56"/>
+      <c r="G50" s="52"/>
+      <c r="H50" s="35" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="31"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="49">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="48"/>
+      <c r="B51" s="48"/>
+      <c r="C51" s="48"/>
+      <c r="D51" s="31">
         <v>37</v>
       </c>
       <c r="E51" s="19">
         <v>0</v>
       </c>
-      <c r="F51" s="43"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="31"/>
-      <c r="B52" s="31"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="49">
+      <c r="F51" s="56"/>
+      <c r="G51" s="52"/>
+      <c r="H51" s="36"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="48"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="31">
         <v>38</v>
       </c>
       <c r="E52" s="19">
         <v>0</v>
       </c>
-      <c r="F52" s="43"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="31"/>
-      <c r="B53" s="31"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="49">
+      <c r="F52" s="56"/>
+      <c r="G52" s="52"/>
+      <c r="H52" s="36"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="48"/>
+      <c r="B53" s="48"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="31">
         <v>64</v>
       </c>
       <c r="E53" s="19">
         <v>0</v>
       </c>
-      <c r="F53" s="43"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="31"/>
-      <c r="B54" s="31"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="49">
+      <c r="F53" s="56"/>
+      <c r="G53" s="52"/>
+      <c r="H53" s="36"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="48"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="31">
         <v>65</v>
       </c>
       <c r="E54" s="19">
         <v>0</v>
       </c>
-      <c r="F54" s="44"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="30" t="s">
+      <c r="F54" s="56"/>
+      <c r="G54" s="52"/>
+      <c r="H54" s="37"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="B55" s="30" t="s">
+      <c r="B55" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="C55" s="30">
+      <c r="C55" s="46">
         <v>29129672</v>
       </c>
-      <c r="D55" s="48">
+      <c r="D55" s="30">
         <v>8</v>
       </c>
       <c r="E55" s="19">
         <v>1777.7650000000001</v>
       </c>
-      <c r="F55" s="35"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="30"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="49">
+      <c r="F55" s="56"/>
+      <c r="G55" s="52"/>
+      <c r="H55" s="38"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="46"/>
+      <c r="B56" s="46"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="31">
         <v>9</v>
       </c>
       <c r="E56" s="19">
         <v>1791.058</v>
       </c>
-      <c r="F56" s="37"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F56" s="56"/>
+      <c r="G56" s="52"/>
+      <c r="H56" s="40"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="28" t="s">
         <v>45</v>
       </c>
@@ -3302,800 +3501,2459 @@
       <c r="C57" s="28">
         <v>288095171</v>
       </c>
-      <c r="D57" s="48">
+      <c r="D57" s="30">
         <v>11</v>
       </c>
       <c r="E57" s="19">
         <v>1.095</v>
       </c>
-      <c r="F57" s="19"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="31" t="s">
+      <c r="F57" s="56"/>
+      <c r="G57" s="52"/>
+      <c r="H57" s="19"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B58" s="31" t="s">
+      <c r="B58" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="C58" s="31">
+      <c r="C58" s="48">
         <v>228758232</v>
       </c>
-      <c r="D58" s="49">
+      <c r="D58" s="31">
         <v>1</v>
       </c>
       <c r="E58" s="19"/>
-      <c r="F58" s="35" t="s">
+      <c r="F58" s="56"/>
+      <c r="G58" s="52"/>
+      <c r="H58" s="38" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="31"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="48">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="48"/>
+      <c r="B59" s="48"/>
+      <c r="C59" s="48"/>
+      <c r="D59" s="30">
         <v>10</v>
       </c>
       <c r="E59" s="19">
         <v>0</v>
       </c>
-      <c r="F59" s="36"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="31"/>
-      <c r="B60" s="31"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="49">
+      <c r="F59" s="56"/>
+      <c r="G59" s="52"/>
+      <c r="H59" s="39"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="48"/>
+      <c r="B60" s="48"/>
+      <c r="C60" s="48"/>
+      <c r="D60" s="31">
         <v>37</v>
       </c>
       <c r="E60" s="19"/>
-      <c r="F60" s="36"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="31"/>
-      <c r="B61" s="31"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="49">
+      <c r="F60" s="56"/>
+      <c r="G60" s="52"/>
+      <c r="H60" s="39"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="48"/>
+      <c r="B61" s="48"/>
+      <c r="C61" s="48"/>
+      <c r="D61" s="31">
         <v>64</v>
       </c>
       <c r="E61" s="19"/>
-      <c r="F61" s="37"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="30" t="s">
+      <c r="F61" s="56"/>
+      <c r="G61" s="52"/>
+      <c r="H61" s="40"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="B62" s="33" t="s">
+      <c r="B62" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="C62" s="30">
+      <c r="C62" s="46">
         <v>13877074</v>
       </c>
-      <c r="D62" s="48">
+      <c r="D62" s="30">
         <v>14</v>
       </c>
       <c r="E62" s="19">
         <v>12.295</v>
       </c>
-      <c r="F62" s="35"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="30"/>
-      <c r="B63" s="33"/>
-      <c r="C63" s="30"/>
-      <c r="D63" s="49">
+      <c r="F62" s="56"/>
+      <c r="G62" s="52"/>
+      <c r="H62" s="38"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="46"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="31">
         <v>15</v>
       </c>
       <c r="E63" s="19">
         <v>7.6189999999999998</v>
       </c>
-      <c r="F63" s="36"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="30"/>
-      <c r="B64" s="33"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="49">
+      <c r="F63" s="56"/>
+      <c r="G63" s="52"/>
+      <c r="H63" s="39"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" s="46"/>
+      <c r="B64" s="49"/>
+      <c r="C64" s="46"/>
+      <c r="D64" s="31">
         <v>41</v>
       </c>
       <c r="E64" s="19">
         <v>12.295</v>
       </c>
-      <c r="F64" s="36"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="30"/>
-      <c r="B65" s="33"/>
-      <c r="C65" s="30"/>
-      <c r="D65" s="49">
+      <c r="F64" s="56"/>
+      <c r="G64" s="52"/>
+      <c r="H64" s="39"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" s="46"/>
+      <c r="B65" s="49"/>
+      <c r="C65" s="46"/>
+      <c r="D65" s="31">
         <v>75</v>
       </c>
       <c r="E65" s="19">
         <v>7.6189999999999998</v>
       </c>
-      <c r="F65" s="36"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="30"/>
-      <c r="B66" s="33"/>
-      <c r="C66" s="30"/>
-      <c r="D66" s="49">
+      <c r="F65" s="56"/>
+      <c r="G65" s="52"/>
+      <c r="H65" s="39"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="46"/>
+      <c r="B66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="31">
         <v>81</v>
       </c>
       <c r="E66" s="19">
         <v>12.295</v>
       </c>
-      <c r="F66" s="36"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="30"/>
-      <c r="B67" s="33"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="49">
+      <c r="F66" s="56"/>
+      <c r="G66" s="52"/>
+      <c r="H66" s="39"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" s="46"/>
+      <c r="B67" s="49"/>
+      <c r="C67" s="46"/>
+      <c r="D67" s="31">
         <v>82</v>
       </c>
       <c r="E67" s="19">
         <v>12.295</v>
       </c>
-      <c r="F67" s="37"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="31" t="s">
+      <c r="F67" s="56"/>
+      <c r="G67" s="52"/>
+      <c r="H67" s="40"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="B68" s="31" t="s">
+      <c r="B68" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="C68" s="31">
+      <c r="C68" s="48">
         <v>126441970</v>
       </c>
-      <c r="D68" s="48">
+      <c r="D68" s="30">
         <v>7</v>
       </c>
       <c r="E68" s="19">
         <v>0</v>
       </c>
-      <c r="F68" s="45" t="s">
+      <c r="F68" s="56"/>
+      <c r="G68" s="52"/>
+      <c r="H68" s="41" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="31"/>
-      <c r="B69" s="31"/>
-      <c r="C69" s="31"/>
-      <c r="D69" s="49">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" s="48"/>
+      <c r="B69" s="48"/>
+      <c r="C69" s="48"/>
+      <c r="D69" s="31">
         <v>34</v>
       </c>
       <c r="E69" s="19"/>
-      <c r="F69" s="46"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="31"/>
-      <c r="B70" s="31"/>
-      <c r="C70" s="31"/>
-      <c r="D70" s="49">
+      <c r="F69" s="56"/>
+      <c r="G69" s="52"/>
+      <c r="H69" s="42"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="48"/>
+      <c r="B70" s="48"/>
+      <c r="C70" s="48"/>
+      <c r="D70" s="31">
         <v>61</v>
       </c>
       <c r="E70" s="19">
         <v>0</v>
       </c>
-      <c r="F70" s="46"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="31"/>
-      <c r="B71" s="31"/>
-      <c r="C71" s="31"/>
-      <c r="D71" s="49">
+      <c r="F70" s="56"/>
+      <c r="G70" s="52"/>
+      <c r="H70" s="42"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="48"/>
+      <c r="B71" s="48"/>
+      <c r="C71" s="48"/>
+      <c r="D71" s="31">
         <v>88</v>
       </c>
       <c r="E71" s="19"/>
-      <c r="F71" s="47"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="32" t="s">
+      <c r="F71" s="56"/>
+      <c r="G71" s="52"/>
+      <c r="H71" s="43"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="B72" s="32" t="s">
+      <c r="B72" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="C72" s="32">
+      <c r="C72" s="47">
         <v>106111735</v>
       </c>
-      <c r="D72" s="48">
+      <c r="D72" s="30">
         <v>14</v>
       </c>
       <c r="E72" s="19">
         <v>0.53300000000000003</v>
       </c>
-      <c r="F72" s="35"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="32"/>
-      <c r="B73" s="32"/>
-      <c r="C73" s="32"/>
-      <c r="D73" s="49">
+      <c r="F72" s="56"/>
+      <c r="G72" s="52"/>
+      <c r="H72" s="38"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" s="47"/>
+      <c r="B73" s="47"/>
+      <c r="C73" s="47"/>
+      <c r="D73" s="31">
         <v>54</v>
       </c>
       <c r="E73" s="19">
         <v>0.53300000000000003</v>
       </c>
-      <c r="F73" s="36"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="32"/>
-      <c r="B74" s="32"/>
-      <c r="C74" s="32"/>
-      <c r="D74" s="49">
+      <c r="F73" s="56"/>
+      <c r="G73" s="52"/>
+      <c r="H73" s="39"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" s="47"/>
+      <c r="B74" s="47"/>
+      <c r="C74" s="47"/>
+      <c r="D74" s="31">
         <v>55</v>
       </c>
       <c r="E74" s="19">
         <v>0.53300000000000003</v>
       </c>
-      <c r="F74" s="36"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="32"/>
-      <c r="B75" s="32"/>
-      <c r="C75" s="32"/>
-      <c r="D75" s="49">
+      <c r="F74" s="56"/>
+      <c r="G74" s="52"/>
+      <c r="H74" s="39"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" s="47"/>
+      <c r="B75" s="47"/>
+      <c r="C75" s="47"/>
+      <c r="D75" s="31">
         <v>74</v>
       </c>
       <c r="E75" s="19">
         <v>0.53300000000000003</v>
       </c>
-      <c r="F75" s="36"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="32"/>
-      <c r="B76" s="32"/>
-      <c r="C76" s="32"/>
-      <c r="D76" s="49">
+      <c r="F75" s="56"/>
+      <c r="G75" s="52"/>
+      <c r="H75" s="39"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" s="47"/>
+      <c r="B76" s="47"/>
+      <c r="C76" s="47"/>
+      <c r="D76" s="31">
         <v>75</v>
       </c>
       <c r="E76" s="19">
         <v>0.53300000000000003</v>
       </c>
-      <c r="F76" s="36"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="32"/>
-      <c r="B77" s="32"/>
-      <c r="C77" s="32"/>
-      <c r="D77" s="49">
+      <c r="F76" s="56"/>
+      <c r="G76" s="52"/>
+      <c r="H76" s="39"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" s="47"/>
+      <c r="B77" s="47"/>
+      <c r="C77" s="47"/>
+      <c r="D77" s="31">
         <v>81</v>
       </c>
       <c r="E77" s="19">
         <v>0.53300000000000003</v>
       </c>
-      <c r="F77" s="36"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="32"/>
-      <c r="B78" s="32"/>
-      <c r="C78" s="32"/>
-      <c r="D78" s="49">
+      <c r="F77" s="56"/>
+      <c r="G77" s="52"/>
+      <c r="H77" s="39"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78" s="47"/>
+      <c r="B78" s="47"/>
+      <c r="C78" s="47"/>
+      <c r="D78" s="31">
         <v>82</v>
       </c>
       <c r="E78" s="19">
         <v>0.53300000000000003</v>
       </c>
-      <c r="F78" s="37"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="31" t="s">
+      <c r="F78" s="56"/>
+      <c r="G78" s="52"/>
+      <c r="H78" s="40"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="B79" s="31" t="s">
+      <c r="B79" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="C79" s="31">
+      <c r="C79" s="48">
         <v>72696935</v>
       </c>
-      <c r="D79" s="48">
+      <c r="D79" s="30">
         <v>19</v>
       </c>
       <c r="E79" s="19">
         <v>0</v>
       </c>
-      <c r="F79" s="39" t="s">
+      <c r="F79" s="56"/>
+      <c r="G79" s="52"/>
+      <c r="H79" s="32" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="31"/>
-      <c r="B80" s="31"/>
-      <c r="C80" s="31"/>
-      <c r="D80" s="49">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80" s="48"/>
+      <c r="B80" s="48"/>
+      <c r="C80" s="48"/>
+      <c r="D80" s="31">
         <v>59</v>
       </c>
       <c r="E80" s="19">
         <v>0.85699999999999998</v>
       </c>
-      <c r="F80" s="40"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="31"/>
-      <c r="B81" s="31"/>
-      <c r="C81" s="31"/>
-      <c r="D81" s="49">
+      <c r="F80" s="56"/>
+      <c r="G80" s="52"/>
+      <c r="H80" s="33"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81" s="48"/>
+      <c r="B81" s="48"/>
+      <c r="C81" s="48"/>
+      <c r="D81" s="31">
         <v>86</v>
       </c>
       <c r="E81" s="19">
         <v>0</v>
       </c>
-      <c r="F81" s="41"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="31" t="s">
+      <c r="F81" s="56"/>
+      <c r="G81" s="52"/>
+      <c r="H81" s="34"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="B82" s="31" t="s">
+      <c r="B82" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="C82" s="31">
+      <c r="C82" s="48">
         <v>337886863</v>
       </c>
-      <c r="D82" s="49">
+      <c r="D82" s="31">
         <v>14</v>
       </c>
       <c r="E82" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="F82" s="42" t="s">
+      <c r="F82" s="57"/>
+      <c r="G82" s="51"/>
+      <c r="H82" s="35" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="31"/>
-      <c r="B83" s="31"/>
-      <c r="C83" s="31"/>
-      <c r="D83" s="49">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83" s="48"/>
+      <c r="B83" s="48"/>
+      <c r="C83" s="48"/>
+      <c r="D83" s="31">
         <v>16</v>
       </c>
       <c r="E83" s="19">
         <v>0</v>
       </c>
-      <c r="F83" s="43"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="31"/>
-      <c r="B84" s="31"/>
-      <c r="C84" s="31"/>
-      <c r="D84" s="49">
+      <c r="F83" s="56"/>
+      <c r="G83" s="52"/>
+      <c r="H83" s="36"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" s="48"/>
+      <c r="B84" s="48"/>
+      <c r="C84" s="48"/>
+      <c r="D84" s="31">
         <v>17</v>
       </c>
       <c r="E84" s="19">
         <v>0</v>
       </c>
-      <c r="F84" s="43"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="31"/>
-      <c r="B85" s="31"/>
-      <c r="C85" s="31"/>
-      <c r="D85" s="49">
+      <c r="F84" s="56"/>
+      <c r="G84" s="52"/>
+      <c r="H84" s="36"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A85" s="48"/>
+      <c r="B85" s="48"/>
+      <c r="C85" s="48"/>
+      <c r="D85" s="31">
         <v>18</v>
       </c>
       <c r="E85" s="19">
         <v>0</v>
       </c>
-      <c r="F85" s="43"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="31"/>
-      <c r="B86" s="31"/>
-      <c r="C86" s="31"/>
-      <c r="D86" s="48">
+      <c r="F85" s="56"/>
+      <c r="G85" s="52"/>
+      <c r="H85" s="36"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86" s="48"/>
+      <c r="B86" s="48"/>
+      <c r="C86" s="48"/>
+      <c r="D86" s="30">
         <v>24</v>
       </c>
       <c r="E86" s="19">
         <v>0</v>
       </c>
-      <c r="F86" s="43"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="31"/>
-      <c r="B87" s="31"/>
-      <c r="C87" s="31"/>
-      <c r="D87" s="49">
+      <c r="F86" s="56"/>
+      <c r="G86" s="52"/>
+      <c r="H86" s="36"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A87" s="48"/>
+      <c r="B87" s="48"/>
+      <c r="C87" s="48"/>
+      <c r="D87" s="31">
         <v>57</v>
       </c>
       <c r="E87" s="19">
         <v>0</v>
       </c>
-      <c r="F87" s="43"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="31"/>
-      <c r="B88" s="31"/>
-      <c r="C88" s="31"/>
-      <c r="D88" s="49">
+      <c r="F87" s="56"/>
+      <c r="G87" s="52"/>
+      <c r="H87" s="36"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88" s="48"/>
+      <c r="B88" s="48"/>
+      <c r="C88" s="48"/>
+      <c r="D88" s="31">
         <v>58</v>
       </c>
       <c r="E88" s="19">
         <v>0</v>
       </c>
-      <c r="F88" s="43"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="31"/>
-      <c r="B89" s="31"/>
-      <c r="C89" s="31"/>
-      <c r="D89" s="49">
+      <c r="F88" s="56"/>
+      <c r="G88" s="52"/>
+      <c r="H88" s="36"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A89" s="48"/>
+      <c r="B89" s="48"/>
+      <c r="C89" s="48"/>
+      <c r="D89" s="31">
         <v>77</v>
       </c>
       <c r="E89" s="19">
         <v>0</v>
       </c>
-      <c r="F89" s="43"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="31"/>
-      <c r="B90" s="31"/>
-      <c r="C90" s="31"/>
-      <c r="D90" s="49">
+      <c r="F89" s="56"/>
+      <c r="G89" s="52"/>
+      <c r="H89" s="36"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A90" s="48"/>
+      <c r="B90" s="48"/>
+      <c r="C90" s="48"/>
+      <c r="D90" s="31">
         <v>78</v>
       </c>
       <c r="E90" s="19">
         <v>0</v>
       </c>
-      <c r="F90" s="43"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="31"/>
-      <c r="B91" s="31"/>
-      <c r="C91" s="31"/>
-      <c r="D91" s="49">
+      <c r="F90" s="56"/>
+      <c r="G90" s="52"/>
+      <c r="H90" s="36"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A91" s="48"/>
+      <c r="B91" s="48"/>
+      <c r="C91" s="48"/>
+      <c r="D91" s="31">
         <v>84</v>
       </c>
       <c r="E91" s="19">
         <v>0</v>
       </c>
-      <c r="F91" s="43"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="31"/>
-      <c r="B92" s="31"/>
-      <c r="C92" s="31"/>
-      <c r="D92" s="49">
+      <c r="F91" s="56"/>
+      <c r="G91" s="52"/>
+      <c r="H91" s="36"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A92" s="48"/>
+      <c r="B92" s="48"/>
+      <c r="C92" s="48"/>
+      <c r="D92" s="31">
         <v>85</v>
       </c>
       <c r="E92" s="19">
         <v>0</v>
       </c>
-      <c r="F92" s="44"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="31" t="s">
+      <c r="F92" s="56"/>
+      <c r="G92" s="52"/>
+      <c r="H92" s="37"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A93" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="B93" s="31" t="s">
+      <c r="B93" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="31">
+      <c r="C93" s="48">
         <v>275420565</v>
       </c>
-      <c r="D93" s="48">
+      <c r="D93" s="30">
         <v>16</v>
       </c>
       <c r="E93" s="19">
         <v>0</v>
       </c>
-      <c r="F93" s="39" t="s">
+      <c r="F93" s="56"/>
+      <c r="G93" s="52"/>
+      <c r="H93" s="32" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="31"/>
-      <c r="B94" s="31"/>
-      <c r="C94" s="31"/>
-      <c r="D94" s="49">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A94" s="48"/>
+      <c r="B94" s="48"/>
+      <c r="C94" s="48"/>
+      <c r="D94" s="31">
         <v>17</v>
       </c>
       <c r="E94" s="19">
         <v>0.71899999999999997</v>
       </c>
-      <c r="F94" s="40"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="31"/>
-      <c r="B95" s="31"/>
-      <c r="C95" s="31"/>
-      <c r="D95" s="49">
+      <c r="F94" s="56"/>
+      <c r="G94" s="52"/>
+      <c r="H94" s="33"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A95" s="48"/>
+      <c r="B95" s="48"/>
+      <c r="C95" s="48"/>
+      <c r="D95" s="31">
         <v>18</v>
       </c>
       <c r="E95" s="19">
         <v>0</v>
       </c>
-      <c r="F95" s="40"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="31"/>
-      <c r="B96" s="31"/>
-      <c r="C96" s="31"/>
-      <c r="D96" s="49">
+      <c r="F95" s="56"/>
+      <c r="G95" s="52"/>
+      <c r="H95" s="33"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A96" s="48"/>
+      <c r="B96" s="48"/>
+      <c r="C96" s="48"/>
+      <c r="D96" s="31">
         <v>24</v>
       </c>
       <c r="E96" s="19">
         <v>0</v>
       </c>
-      <c r="F96" s="40"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="31"/>
-      <c r="B97" s="31"/>
-      <c r="C97" s="31"/>
-      <c r="D97" s="49">
+      <c r="F96" s="56"/>
+      <c r="G96" s="52"/>
+      <c r="H96" s="33"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A97" s="48"/>
+      <c r="B97" s="48"/>
+      <c r="C97" s="48"/>
+      <c r="D97" s="31">
         <v>56</v>
       </c>
       <c r="E97" s="19">
         <v>0</v>
       </c>
-      <c r="F97" s="40"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="31"/>
-      <c r="B98" s="31"/>
-      <c r="C98" s="31"/>
-      <c r="D98" s="49">
+      <c r="F97" s="56"/>
+      <c r="G97" s="52"/>
+      <c r="H97" s="33"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A98" s="48"/>
+      <c r="B98" s="48"/>
+      <c r="C98" s="48"/>
+      <c r="D98" s="31">
         <v>58</v>
       </c>
       <c r="E98" s="19">
         <v>0</v>
       </c>
-      <c r="F98" s="40"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="31"/>
-      <c r="B99" s="31"/>
-      <c r="C99" s="31"/>
-      <c r="D99" s="49">
+      <c r="F98" s="56"/>
+      <c r="G98" s="52"/>
+      <c r="H98" s="33"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A99" s="48"/>
+      <c r="B99" s="48"/>
+      <c r="C99" s="48"/>
+      <c r="D99" s="31">
         <v>76</v>
       </c>
       <c r="E99" s="19">
         <v>0</v>
       </c>
-      <c r="F99" s="40"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="31"/>
-      <c r="B100" s="31"/>
-      <c r="C100" s="31"/>
-      <c r="D100" s="49">
+      <c r="F99" s="56"/>
+      <c r="G99" s="52"/>
+      <c r="H99" s="33"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A100" s="48"/>
+      <c r="B100" s="48"/>
+      <c r="C100" s="48"/>
+      <c r="D100" s="31">
         <v>77</v>
       </c>
       <c r="E100" s="19">
         <v>0</v>
       </c>
-      <c r="F100" s="40"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="31"/>
-      <c r="B101" s="31"/>
-      <c r="C101" s="31"/>
-      <c r="D101" s="49">
+      <c r="F100" s="56"/>
+      <c r="G100" s="52"/>
+      <c r="H100" s="33"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A101" s="48"/>
+      <c r="B101" s="48"/>
+      <c r="C101" s="48"/>
+      <c r="D101" s="31">
         <v>78</v>
       </c>
       <c r="E101" s="19">
         <v>0</v>
       </c>
-      <c r="F101" s="40"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" s="31"/>
-      <c r="B102" s="31"/>
-      <c r="C102" s="31"/>
-      <c r="D102" s="49">
+      <c r="F101" s="56"/>
+      <c r="G101" s="52"/>
+      <c r="H101" s="33"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" s="48"/>
+      <c r="B102" s="48"/>
+      <c r="C102" s="48"/>
+      <c r="D102" s="31">
         <v>83</v>
       </c>
       <c r="E102" s="19">
         <v>0</v>
       </c>
-      <c r="F102" s="40"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" s="31"/>
-      <c r="B103" s="31"/>
-      <c r="C103" s="31"/>
-      <c r="D103" s="49">
+      <c r="F102" s="56"/>
+      <c r="G102" s="52"/>
+      <c r="H102" s="33"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A103" s="48"/>
+      <c r="B103" s="48"/>
+      <c r="C103" s="48"/>
+      <c r="D103" s="31">
         <v>85</v>
       </c>
       <c r="E103" s="19">
         <v>0</v>
       </c>
-      <c r="F103" s="41"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" s="30" t="s">
+      <c r="F103" s="56"/>
+      <c r="G103" s="52"/>
+      <c r="H103" s="34"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A104" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="B104" s="30" t="s">
+      <c r="B104" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="C104" s="30">
+      <c r="C104" s="46">
         <v>180730928</v>
       </c>
-      <c r="D104" s="49">
+      <c r="D104" s="31">
         <v>1</v>
       </c>
       <c r="E104" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="F104" s="35"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A105" s="30"/>
-      <c r="B105" s="30"/>
-      <c r="C105" s="30"/>
-      <c r="D105" s="48">
+      <c r="F104" s="57"/>
+      <c r="G104" s="51"/>
+      <c r="H104" s="38"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A105" s="46"/>
+      <c r="B105" s="46"/>
+      <c r="C105" s="46"/>
+      <c r="D105" s="30">
         <v>8</v>
       </c>
       <c r="E105" s="19">
         <v>7078.9560000000001</v>
       </c>
-      <c r="F105" s="36"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" s="30"/>
-      <c r="B106" s="30"/>
-      <c r="C106" s="30"/>
-      <c r="D106" s="49">
+      <c r="F105" s="56"/>
+      <c r="G105" s="52"/>
+      <c r="H105" s="39"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A106" s="46"/>
+      <c r="B106" s="46"/>
+      <c r="C106" s="46"/>
+      <c r="D106" s="31">
         <v>61</v>
       </c>
       <c r="E106" s="19">
         <v>7078.9560000000001</v>
       </c>
-      <c r="F106" s="36"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A107" s="30"/>
-      <c r="B107" s="30"/>
-      <c r="C107" s="30"/>
-      <c r="D107" s="49">
+      <c r="F106" s="56"/>
+      <c r="G106" s="52"/>
+      <c r="H106" s="39"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A107" s="46"/>
+      <c r="B107" s="46"/>
+      <c r="C107" s="46"/>
+      <c r="D107" s="31">
         <v>62</v>
       </c>
       <c r="E107" s="19">
         <v>7078.9560000000001</v>
       </c>
-      <c r="F107" s="37"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A108" s="31" t="s">
+      <c r="F107" s="56"/>
+      <c r="G107" s="52"/>
+      <c r="H107" s="40"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A108" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="B108" s="31" t="s">
+      <c r="B108" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="C108" s="31">
+      <c r="C108" s="48">
         <v>143681075</v>
       </c>
-      <c r="D108" s="48">
+      <c r="D108" s="30">
         <v>19</v>
       </c>
       <c r="E108" s="19">
         <v>0</v>
       </c>
-      <c r="F108" s="42" t="s">
+      <c r="F108" s="56"/>
+      <c r="G108" s="52"/>
+      <c r="H108" s="35" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A109" s="31"/>
-      <c r="B109" s="31"/>
-      <c r="C109" s="31"/>
-      <c r="D109" s="49">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A109" s="48"/>
+      <c r="B109" s="48"/>
+      <c r="C109" s="48"/>
+      <c r="D109" s="31">
         <v>59</v>
       </c>
       <c r="E109" s="19">
         <v>0</v>
       </c>
-      <c r="F109" s="43"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A110" s="31"/>
-      <c r="B110" s="31"/>
-      <c r="C110" s="31"/>
-      <c r="D110" s="49">
+      <c r="F109" s="56"/>
+      <c r="G109" s="52"/>
+      <c r="H109" s="36"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A110" s="48"/>
+      <c r="B110" s="48"/>
+      <c r="C110" s="48"/>
+      <c r="D110" s="31">
         <v>73</v>
       </c>
       <c r="E110" s="19">
         <v>0</v>
       </c>
-      <c r="F110" s="43"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111" s="31"/>
-      <c r="B111" s="31"/>
-      <c r="C111" s="31"/>
-      <c r="D111" s="49">
+      <c r="F110" s="56"/>
+      <c r="G110" s="52"/>
+      <c r="H110" s="36"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A111" s="48"/>
+      <c r="B111" s="48"/>
+      <c r="C111" s="48"/>
+      <c r="D111" s="31">
         <v>86</v>
       </c>
       <c r="E111" s="19">
         <v>0</v>
       </c>
-      <c r="F111" s="44"/>
+      <c r="F111" s="56"/>
+      <c r="G111" s="52"/>
+      <c r="H111" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="F79:F81"/>
-    <mergeCell ref="F82:F92"/>
-    <mergeCell ref="F93:F103"/>
-    <mergeCell ref="F104:F107"/>
-    <mergeCell ref="F108:F111"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="F58:F61"/>
-    <mergeCell ref="F62:F67"/>
-    <mergeCell ref="F68:F71"/>
-    <mergeCell ref="F72:F78"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="F30:F34"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="F38:F49"/>
-    <mergeCell ref="F50:F54"/>
-    <mergeCell ref="F10:F19"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="B104:B107"/>
+    <mergeCell ref="C104:C107"/>
+    <mergeCell ref="C108:C111"/>
+    <mergeCell ref="B108:B111"/>
+    <mergeCell ref="A108:A111"/>
+    <mergeCell ref="C82:C92"/>
+    <mergeCell ref="B82:B92"/>
+    <mergeCell ref="A82:A92"/>
+    <mergeCell ref="C93:C103"/>
+    <mergeCell ref="B93:B103"/>
+    <mergeCell ref="A93:A103"/>
+    <mergeCell ref="C72:C78"/>
+    <mergeCell ref="B72:B78"/>
+    <mergeCell ref="A72:A78"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="C62:C67"/>
+    <mergeCell ref="B62:B67"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="C38:C49"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="B50:B54"/>
+    <mergeCell ref="C50:C54"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A10:A19"/>
+    <mergeCell ref="B10:B19"/>
+    <mergeCell ref="C10:C19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:C9"/>
-    <mergeCell ref="A10:A19"/>
-    <mergeCell ref="B10:B19"/>
-    <mergeCell ref="C10:C19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="H10:H19"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="H30:H34"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="H38:H49"/>
+    <mergeCell ref="H50:H54"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="H58:H61"/>
+    <mergeCell ref="H62:H67"/>
+    <mergeCell ref="H68:H71"/>
+    <mergeCell ref="H72:H78"/>
+    <mergeCell ref="H79:H81"/>
+    <mergeCell ref="H82:H92"/>
+    <mergeCell ref="H93:H103"/>
+    <mergeCell ref="H104:H107"/>
+    <mergeCell ref="H108:H111"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60225743-A402-4A5B-8885-503171F5619A}">
+  <dimension ref="A1:F141"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="45">
+        <v>75311623</v>
+      </c>
+      <c r="D2" s="18">
+        <v>1</v>
+      </c>
+      <c r="E2" s="68" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="59">
+        <v>5.2398300000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="19">
+        <v>8</v>
+      </c>
+      <c r="E3" s="52">
+        <v>4.8378704952425302</v>
+      </c>
+      <c r="F3" s="60"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="22">
+        <v>9</v>
+      </c>
+      <c r="E4" s="50">
+        <v>4.8727570024205704</v>
+      </c>
+      <c r="F4" s="60"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="69" t="s">
+        <v>163</v>
+      </c>
+      <c r="E5" s="56">
+        <v>5.0664257843651503</v>
+      </c>
+      <c r="F5" s="61"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="29">
+        <v>49720925</v>
+      </c>
+      <c r="D6" s="30">
+        <v>18</v>
+      </c>
+      <c r="E6" s="56">
+        <v>1.4693681092036801</v>
+      </c>
+      <c r="F6" s="66">
+        <v>1.4510099999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="47">
+        <v>435781776</v>
+      </c>
+      <c r="D7" s="30">
+        <v>14</v>
+      </c>
+      <c r="E7" s="56">
+        <v>0.67124809679754605</v>
+      </c>
+      <c r="F7" s="62">
+        <v>0.67753300000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="31">
+        <v>41</v>
+      </c>
+      <c r="E8" s="56">
+        <v>0.68175980018525995</v>
+      </c>
+      <c r="F8" s="60"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="31">
+        <v>54</v>
+      </c>
+      <c r="E9" s="56">
+        <v>0.67254816493406</v>
+      </c>
+      <c r="F9" s="60"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="31">
+        <v>81</v>
+      </c>
+      <c r="E10" s="56">
+        <v>0.68265733283112395</v>
+      </c>
+      <c r="F10" s="60"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="47"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="69" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" s="56">
+        <v>0.67659925236799101</v>
+      </c>
+      <c r="F11" s="61"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="48">
+        <v>434408053</v>
+      </c>
+      <c r="D12" s="31">
+        <v>1</v>
+      </c>
+      <c r="E12" s="68" t="s">
+        <v>155</v>
+      </c>
+      <c r="F12" s="62">
+        <v>7.3338000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="48"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="31">
+        <v>2</v>
+      </c>
+      <c r="E13" s="68" t="s">
+        <v>155</v>
+      </c>
+      <c r="F13" s="60"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="48"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="30">
+        <v>6</v>
+      </c>
+      <c r="E14" s="56">
+        <v>7.2573903349586999</v>
+      </c>
+      <c r="F14" s="60"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="48"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="31">
+        <v>33</v>
+      </c>
+      <c r="E15" s="56">
+        <v>6.4596552346367799</v>
+      </c>
+      <c r="F15" s="60"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="48"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="31">
+        <v>43</v>
+      </c>
+      <c r="E16" s="56">
+        <v>8.0956872768653394</v>
+      </c>
+      <c r="F16" s="60"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="48"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="31">
+        <v>44</v>
+      </c>
+      <c r="E17" s="56">
+        <v>8.0520759460678093</v>
+      </c>
+      <c r="F17" s="60"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="48"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="31">
+        <v>45</v>
+      </c>
+      <c r="E18" s="56">
+        <v>8.1837988587493093</v>
+      </c>
+      <c r="F18" s="60"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="48"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="31">
+        <v>71</v>
+      </c>
+      <c r="E19" s="56">
+        <v>8.1071427208107707</v>
+      </c>
+      <c r="F19" s="60"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="48"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="31">
+        <v>72</v>
+      </c>
+      <c r="E20" s="56">
+        <v>7.9142851697268499</v>
+      </c>
+      <c r="F20" s="60"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="48"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="31">
+        <v>87</v>
+      </c>
+      <c r="E21" s="56">
+        <v>4.7820233275211601</v>
+      </c>
+      <c r="F21" s="60"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="48"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="69" t="s">
+        <v>163</v>
+      </c>
+      <c r="E22" s="56">
+        <v>7.4269915443075902</v>
+      </c>
+      <c r="F22" s="61"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="58" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="58">
+        <v>329074395</v>
+      </c>
+      <c r="D23" s="30">
+        <v>15</v>
+      </c>
+      <c r="E23" s="56"/>
+      <c r="F23" s="62">
+        <v>3.7668200000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="58"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="31">
+        <v>16</v>
+      </c>
+      <c r="E24" s="56"/>
+      <c r="F24" s="60"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="58"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="31">
+        <v>17</v>
+      </c>
+      <c r="E25" s="56"/>
+      <c r="F25" s="60"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="58"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="31">
+        <v>84</v>
+      </c>
+      <c r="E26" s="56"/>
+      <c r="F26" s="61"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="48">
+        <v>316493106</v>
+      </c>
+      <c r="D27" s="30">
+        <v>24</v>
+      </c>
+      <c r="E27" s="56"/>
+      <c r="F27" s="62">
+        <v>4.6325000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="48"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="31">
+        <v>25</v>
+      </c>
+      <c r="E28" s="56"/>
+      <c r="F28" s="60"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="48"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="31">
+        <v>26</v>
+      </c>
+      <c r="E29" s="56"/>
+      <c r="F29" s="61"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="47">
+        <v>304996702</v>
+      </c>
+      <c r="D30" s="30">
+        <v>10</v>
+      </c>
+      <c r="E30" s="56"/>
+      <c r="F30" s="62">
+        <v>1.4137900000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="47"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="31">
+        <v>11</v>
+      </c>
+      <c r="E31" s="56"/>
+      <c r="F31" s="60"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="47"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="31">
+        <v>90</v>
+      </c>
+      <c r="E32" s="56"/>
+      <c r="F32" s="61"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="48">
+        <v>302824830</v>
+      </c>
+      <c r="D33" s="30">
+        <v>6</v>
+      </c>
+      <c r="E33" s="56"/>
+      <c r="F33" s="62">
+        <v>3.2718099999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="48"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="31">
+        <v>43</v>
+      </c>
+      <c r="E34" s="56"/>
+      <c r="F34" s="60"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="48"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="31">
+        <v>44</v>
+      </c>
+      <c r="E35" s="56"/>
+      <c r="F35" s="60"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="48"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="31">
+        <v>45</v>
+      </c>
+      <c r="E36" s="56"/>
+      <c r="F36" s="60"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="48"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="31">
+        <v>71</v>
+      </c>
+      <c r="E37" s="56"/>
+      <c r="F37" s="61"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="47">
+        <v>284141111</v>
+      </c>
+      <c r="D38" s="31">
+        <v>17</v>
+      </c>
+      <c r="E38" s="56"/>
+      <c r="F38" s="62">
+        <v>0.62248000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="47"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="30">
+        <v>18</v>
+      </c>
+      <c r="E39" s="56"/>
+      <c r="F39" s="60"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="47"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="31">
+        <v>85</v>
+      </c>
+      <c r="E40" s="56"/>
+      <c r="F40" s="61"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="48">
+        <v>277502552</v>
+      </c>
+      <c r="D41" s="31">
+        <v>14</v>
+      </c>
+      <c r="E41" s="57"/>
+      <c r="F41" s="62">
+        <v>0.91777200000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="48"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="31">
+        <v>15</v>
+      </c>
+      <c r="E42" s="56"/>
+      <c r="F42" s="60"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="48"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="30">
+        <v>16</v>
+      </c>
+      <c r="E43" s="56"/>
+      <c r="F43" s="60"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="48"/>
+      <c r="B44" s="48"/>
+      <c r="C44" s="48"/>
+      <c r="D44" s="31">
+        <v>17</v>
+      </c>
+      <c r="E44" s="56"/>
+      <c r="F44" s="60"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="48"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="31">
+        <v>55</v>
+      </c>
+      <c r="E45" s="56"/>
+      <c r="F45" s="60"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="48"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="31">
+        <v>56</v>
+      </c>
+      <c r="E46" s="56"/>
+      <c r="F46" s="60"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="48"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="31">
+        <v>57</v>
+      </c>
+      <c r="E47" s="56"/>
+      <c r="F47" s="60"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="48"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="31">
+        <v>75</v>
+      </c>
+      <c r="E48" s="56"/>
+      <c r="F48" s="60"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="48"/>
+      <c r="B49" s="48"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="31">
+        <v>76</v>
+      </c>
+      <c r="E49" s="56"/>
+      <c r="F49" s="60"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="48"/>
+      <c r="B50" s="48"/>
+      <c r="C50" s="48"/>
+      <c r="D50" s="31">
+        <v>77</v>
+      </c>
+      <c r="E50" s="56"/>
+      <c r="F50" s="60"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="48"/>
+      <c r="B51" s="48"/>
+      <c r="C51" s="48"/>
+      <c r="D51" s="31">
+        <v>82</v>
+      </c>
+      <c r="E51" s="56"/>
+      <c r="F51" s="60"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="48"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="31">
+        <v>84</v>
+      </c>
+      <c r="E52" s="56"/>
+      <c r="F52" s="61"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="48">
+        <v>310883625</v>
+      </c>
+      <c r="D53" s="30">
+        <v>11</v>
+      </c>
+      <c r="E53" s="56"/>
+      <c r="F53" s="62">
+        <v>6.6766399999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="48"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="31">
+        <v>37</v>
+      </c>
+      <c r="E54" s="56"/>
+      <c r="F54" s="60"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="48"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="31">
+        <v>38</v>
+      </c>
+      <c r="E55" s="56"/>
+      <c r="F55" s="60"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="48"/>
+      <c r="B56" s="48"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="31">
+        <v>64</v>
+      </c>
+      <c r="E56" s="56"/>
+      <c r="F56" s="60"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="48"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="31">
+        <v>65</v>
+      </c>
+      <c r="E57" s="56"/>
+      <c r="F57" s="61"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" s="46">
+        <v>29129672</v>
+      </c>
+      <c r="D58" s="30">
+        <v>8</v>
+      </c>
+      <c r="E58" s="56"/>
+      <c r="F58" s="62">
+        <v>6.9884599999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="46"/>
+      <c r="B59" s="46"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="31">
+        <v>9</v>
+      </c>
+      <c r="E59" s="56"/>
+      <c r="F59" s="61"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B60" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C60" s="28">
+        <v>288095171</v>
+      </c>
+      <c r="D60" s="30">
+        <v>11</v>
+      </c>
+      <c r="E60" s="56"/>
+      <c r="F60" s="66">
+        <v>12.1547</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B61" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" s="48">
+        <v>228758232</v>
+      </c>
+      <c r="D61" s="31">
+        <v>1</v>
+      </c>
+      <c r="E61" s="56"/>
+      <c r="F61" s="62">
+        <v>10.144299999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="48"/>
+      <c r="B62" s="48"/>
+      <c r="C62" s="48"/>
+      <c r="D62" s="30">
+        <v>10</v>
+      </c>
+      <c r="E62" s="56"/>
+      <c r="F62" s="60"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="48"/>
+      <c r="B63" s="48"/>
+      <c r="C63" s="48"/>
+      <c r="D63" s="31">
+        <v>37</v>
+      </c>
+      <c r="E63" s="56"/>
+      <c r="F63" s="60"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="48"/>
+      <c r="B64" s="48"/>
+      <c r="C64" s="48"/>
+      <c r="D64" s="31">
+        <v>64</v>
+      </c>
+      <c r="E64" s="56"/>
+      <c r="F64" s="61"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B65" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C65" s="46">
+        <v>13877074</v>
+      </c>
+      <c r="D65" s="30">
+        <v>14</v>
+      </c>
+      <c r="E65" s="56"/>
+      <c r="F65" s="62">
+        <v>10.925000000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="46"/>
+      <c r="B66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="31">
+        <v>15</v>
+      </c>
+      <c r="E66" s="56"/>
+      <c r="F66" s="60"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="46"/>
+      <c r="B67" s="49"/>
+      <c r="C67" s="46"/>
+      <c r="D67" s="31">
+        <v>41</v>
+      </c>
+      <c r="E67" s="56"/>
+      <c r="F67" s="60"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="46"/>
+      <c r="B68" s="49"/>
+      <c r="C68" s="46"/>
+      <c r="D68" s="31">
+        <v>75</v>
+      </c>
+      <c r="E68" s="56"/>
+      <c r="F68" s="60"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="46"/>
+      <c r="B69" s="49"/>
+      <c r="C69" s="46"/>
+      <c r="D69" s="31">
+        <v>81</v>
+      </c>
+      <c r="E69" s="56"/>
+      <c r="F69" s="60"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="46"/>
+      <c r="B70" s="49"/>
+      <c r="C70" s="46"/>
+      <c r="D70" s="31">
+        <v>82</v>
+      </c>
+      <c r="E70" s="56"/>
+      <c r="F70" s="61"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B71" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="C71" s="48">
+        <v>126441970</v>
+      </c>
+      <c r="D71" s="30">
+        <v>7</v>
+      </c>
+      <c r="E71" s="56"/>
+      <c r="F71" s="63">
+        <v>7.1592200000000004</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="48"/>
+      <c r="B72" s="48"/>
+      <c r="C72" s="48"/>
+      <c r="D72" s="31">
+        <v>34</v>
+      </c>
+      <c r="E72" s="56"/>
+      <c r="F72" s="64"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="48"/>
+      <c r="B73" s="48"/>
+      <c r="C73" s="48"/>
+      <c r="D73" s="31">
+        <v>61</v>
+      </c>
+      <c r="E73" s="56"/>
+      <c r="F73" s="64"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="48"/>
+      <c r="B74" s="48"/>
+      <c r="C74" s="48"/>
+      <c r="D74" s="31">
+        <v>88</v>
+      </c>
+      <c r="E74" s="56"/>
+      <c r="F74" s="65"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B75" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="C75" s="47">
+        <v>106111735</v>
+      </c>
+      <c r="D75" s="30">
+        <v>14</v>
+      </c>
+      <c r="E75" s="56"/>
+      <c r="F75" s="62">
+        <v>7.3662099999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="47"/>
+      <c r="B76" s="47"/>
+      <c r="C76" s="47"/>
+      <c r="D76" s="31">
+        <v>54</v>
+      </c>
+      <c r="E76" s="56"/>
+      <c r="F76" s="60"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="47"/>
+      <c r="B77" s="47"/>
+      <c r="C77" s="47"/>
+      <c r="D77" s="31">
+        <v>55</v>
+      </c>
+      <c r="E77" s="56"/>
+      <c r="F77" s="60"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="47"/>
+      <c r="B78" s="47"/>
+      <c r="C78" s="47"/>
+      <c r="D78" s="31">
+        <v>74</v>
+      </c>
+      <c r="E78" s="56"/>
+      <c r="F78" s="60"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="47"/>
+      <c r="B79" s="47"/>
+      <c r="C79" s="47"/>
+      <c r="D79" s="31">
+        <v>75</v>
+      </c>
+      <c r="E79" s="56"/>
+      <c r="F79" s="60"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="47"/>
+      <c r="B80" s="47"/>
+      <c r="C80" s="47"/>
+      <c r="D80" s="31">
+        <v>81</v>
+      </c>
+      <c r="E80" s="56"/>
+      <c r="F80" s="60"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="47"/>
+      <c r="B81" s="47"/>
+      <c r="C81" s="47"/>
+      <c r="D81" s="31">
+        <v>82</v>
+      </c>
+      <c r="E81" s="56"/>
+      <c r="F81" s="61"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="B82" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="C82" s="58">
+        <v>72696935</v>
+      </c>
+      <c r="D82" s="30">
+        <v>19</v>
+      </c>
+      <c r="E82" s="56"/>
+      <c r="F82" s="62">
+        <v>0.543462</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="58"/>
+      <c r="B83" s="58"/>
+      <c r="C83" s="58"/>
+      <c r="D83" s="31">
+        <v>59</v>
+      </c>
+      <c r="E83" s="56"/>
+      <c r="F83" s="60"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="58"/>
+      <c r="B84" s="58"/>
+      <c r="C84" s="58"/>
+      <c r="D84" s="31">
+        <v>86</v>
+      </c>
+      <c r="E84" s="56"/>
+      <c r="F84" s="61"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B85" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="C85" s="48">
+        <v>337886863</v>
+      </c>
+      <c r="D85" s="31">
+        <v>14</v>
+      </c>
+      <c r="E85" s="57"/>
+      <c r="F85" s="62">
+        <v>5.7008099999999997</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" s="48"/>
+      <c r="B86" s="48"/>
+      <c r="C86" s="48"/>
+      <c r="D86" s="31">
+        <v>16</v>
+      </c>
+      <c r="E86" s="56"/>
+      <c r="F86" s="60"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" s="48"/>
+      <c r="B87" s="48"/>
+      <c r="C87" s="48"/>
+      <c r="D87" s="31">
+        <v>17</v>
+      </c>
+      <c r="E87" s="56"/>
+      <c r="F87" s="60"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" s="48"/>
+      <c r="B88" s="48"/>
+      <c r="C88" s="48"/>
+      <c r="D88" s="31">
+        <v>18</v>
+      </c>
+      <c r="E88" s="56"/>
+      <c r="F88" s="60"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" s="48"/>
+      <c r="B89" s="48"/>
+      <c r="C89" s="48"/>
+      <c r="D89" s="30">
+        <v>24</v>
+      </c>
+      <c r="E89" s="56"/>
+      <c r="F89" s="60"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" s="48"/>
+      <c r="B90" s="48"/>
+      <c r="C90" s="48"/>
+      <c r="D90" s="31">
+        <v>57</v>
+      </c>
+      <c r="E90" s="56"/>
+      <c r="F90" s="60"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" s="48"/>
+      <c r="B91" s="48"/>
+      <c r="C91" s="48"/>
+      <c r="D91" s="31">
+        <v>58</v>
+      </c>
+      <c r="E91" s="56"/>
+      <c r="F91" s="60"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" s="48"/>
+      <c r="B92" s="48"/>
+      <c r="C92" s="48"/>
+      <c r="D92" s="31">
+        <v>77</v>
+      </c>
+      <c r="E92" s="56"/>
+      <c r="F92" s="60"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" s="48"/>
+      <c r="B93" s="48"/>
+      <c r="C93" s="48"/>
+      <c r="D93" s="31">
+        <v>78</v>
+      </c>
+      <c r="E93" s="56"/>
+      <c r="F93" s="60"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" s="48"/>
+      <c r="B94" s="48"/>
+      <c r="C94" s="48"/>
+      <c r="D94" s="31">
+        <v>84</v>
+      </c>
+      <c r="E94" s="56"/>
+      <c r="F94" s="60"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" s="48"/>
+      <c r="B95" s="48"/>
+      <c r="C95" s="48"/>
+      <c r="D95" s="31">
+        <v>85</v>
+      </c>
+      <c r="E95" s="56"/>
+      <c r="F95" s="61"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="B96" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="C96" s="58">
+        <v>275420565</v>
+      </c>
+      <c r="D96" s="30">
+        <v>16</v>
+      </c>
+      <c r="E96" s="56"/>
+      <c r="F96" s="62">
+        <v>1.6960599999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" s="58"/>
+      <c r="B97" s="58"/>
+      <c r="C97" s="58"/>
+      <c r="D97" s="31">
+        <v>17</v>
+      </c>
+      <c r="E97" s="56"/>
+      <c r="F97" s="60"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" s="58"/>
+      <c r="B98" s="58"/>
+      <c r="C98" s="58"/>
+      <c r="D98" s="31">
+        <v>18</v>
+      </c>
+      <c r="E98" s="56"/>
+      <c r="F98" s="60"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" s="58"/>
+      <c r="B99" s="58"/>
+      <c r="C99" s="58"/>
+      <c r="D99" s="31">
+        <v>24</v>
+      </c>
+      <c r="E99" s="56"/>
+      <c r="F99" s="60"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" s="58"/>
+      <c r="B100" s="58"/>
+      <c r="C100" s="58"/>
+      <c r="D100" s="31">
+        <v>56</v>
+      </c>
+      <c r="E100" s="56"/>
+      <c r="F100" s="60"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" s="58"/>
+      <c r="B101" s="58"/>
+      <c r="C101" s="58"/>
+      <c r="D101" s="31">
+        <v>58</v>
+      </c>
+      <c r="E101" s="56"/>
+      <c r="F101" s="60"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" s="58"/>
+      <c r="B102" s="58"/>
+      <c r="C102" s="58"/>
+      <c r="D102" s="31">
+        <v>76</v>
+      </c>
+      <c r="E102" s="56"/>
+      <c r="F102" s="60"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" s="58"/>
+      <c r="B103" s="58"/>
+      <c r="C103" s="58"/>
+      <c r="D103" s="31">
+        <v>77</v>
+      </c>
+      <c r="E103" s="56"/>
+      <c r="F103" s="60"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" s="58"/>
+      <c r="B104" s="58"/>
+      <c r="C104" s="58"/>
+      <c r="D104" s="31">
+        <v>78</v>
+      </c>
+      <c r="E104" s="56"/>
+      <c r="F104" s="60"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" s="58"/>
+      <c r="B105" s="58"/>
+      <c r="C105" s="58"/>
+      <c r="D105" s="31">
+        <v>83</v>
+      </c>
+      <c r="E105" s="56"/>
+      <c r="F105" s="60"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" s="58"/>
+      <c r="B106" s="58"/>
+      <c r="C106" s="58"/>
+      <c r="D106" s="31">
+        <v>85</v>
+      </c>
+      <c r="E106" s="56"/>
+      <c r="F106" s="61"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="B107" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C107" s="46">
+        <v>180730928</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1</v>
+      </c>
+      <c r="E107" s="57"/>
+      <c r="F107" s="62">
+        <v>0.56733900000000004</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" s="46"/>
+      <c r="B108" s="46"/>
+      <c r="C108" s="46"/>
+      <c r="D108" s="30">
+        <v>8</v>
+      </c>
+      <c r="E108" s="56"/>
+      <c r="F108" s="60"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" s="46"/>
+      <c r="B109" s="46"/>
+      <c r="C109" s="46"/>
+      <c r="D109" s="31">
+        <v>61</v>
+      </c>
+      <c r="E109" s="56"/>
+      <c r="F109" s="60"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" s="46"/>
+      <c r="B110" s="46"/>
+      <c r="C110" s="46"/>
+      <c r="D110" s="31">
+        <v>62</v>
+      </c>
+      <c r="E110" s="56"/>
+      <c r="F110" s="61"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B111" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="C111" s="48">
+        <v>143681075</v>
+      </c>
+      <c r="D111" s="30">
+        <v>19</v>
+      </c>
+      <c r="E111" s="56"/>
+      <c r="F111" s="62">
+        <v>1.33982</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" s="48"/>
+      <c r="B112" s="48"/>
+      <c r="C112" s="48"/>
+      <c r="D112" s="31">
+        <v>59</v>
+      </c>
+      <c r="E112" s="56"/>
+      <c r="F112" s="60"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" s="48"/>
+      <c r="B113" s="48"/>
+      <c r="C113" s="48"/>
+      <c r="D113" s="31">
+        <v>73</v>
+      </c>
+      <c r="E113" s="56"/>
+      <c r="F113" s="60"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" s="48"/>
+      <c r="B114" s="48"/>
+      <c r="C114" s="48"/>
+      <c r="D114" s="31">
+        <v>86</v>
+      </c>
+      <c r="E114" s="56"/>
+      <c r="F114" s="61"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F115" s="67"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F116" s="67"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F117" s="67"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F118" s="67"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F119" s="67"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F120" s="67"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F121" s="67"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F122" s="67"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F123" s="67"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F124" s="67"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F125" s="67"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F126" s="67"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F127" s="67"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F128" s="67"/>
+    </row>
+    <row r="129" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F129" s="67"/>
+    </row>
+    <row r="130" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F130" s="67"/>
+    </row>
+    <row r="131" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F131" s="67"/>
+    </row>
+    <row r="132" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F132" s="67"/>
+    </row>
+    <row r="133" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F133" s="67"/>
+    </row>
+    <row r="134" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F134" s="67"/>
+    </row>
+    <row r="135" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F135" s="67"/>
+    </row>
+    <row r="136" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F136" s="67"/>
+    </row>
+    <row r="137" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F137" s="67"/>
+    </row>
+    <row r="138" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F138" s="67"/>
+    </row>
+    <row r="139" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F139" s="67"/>
+    </row>
+    <row r="140" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F140" s="67"/>
+    </row>
+    <row r="141" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F141" s="67"/>
+    </row>
+  </sheetData>
+  <mergeCells count="80">
+    <mergeCell ref="A107:A110"/>
+    <mergeCell ref="B107:B110"/>
+    <mergeCell ref="C107:C110"/>
+    <mergeCell ref="F107:F110"/>
+    <mergeCell ref="A111:A114"/>
+    <mergeCell ref="B111:B114"/>
+    <mergeCell ref="C111:C114"/>
+    <mergeCell ref="F111:F114"/>
+    <mergeCell ref="A85:A95"/>
+    <mergeCell ref="B85:B95"/>
+    <mergeCell ref="C85:C95"/>
+    <mergeCell ref="F85:F95"/>
+    <mergeCell ref="A96:A106"/>
+    <mergeCell ref="B96:B106"/>
+    <mergeCell ref="C96:C106"/>
+    <mergeCell ref="F96:F106"/>
+    <mergeCell ref="A75:A81"/>
+    <mergeCell ref="B75:B81"/>
+    <mergeCell ref="C75:C81"/>
+    <mergeCell ref="F75:F81"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="C82:C84"/>
+    <mergeCell ref="F82:F84"/>
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="B65:B70"/>
+    <mergeCell ref="C65:C70"/>
+    <mergeCell ref="F65:F70"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="F71:F74"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="C61:C64"/>
+    <mergeCell ref="F61:F64"/>
+    <mergeCell ref="A41:A52"/>
+    <mergeCell ref="B41:B52"/>
+    <mergeCell ref="C41:C52"/>
+    <mergeCell ref="F41:F52"/>
+    <mergeCell ref="A53:A57"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="C53:C57"/>
+    <mergeCell ref="F53:F57"/>
+    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="B33:B37"/>
+    <mergeCell ref="C33:C37"/>
+    <mergeCell ref="F33:F37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
     <mergeCell ref="C27:C29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="C38:C49"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="B50:B54"/>
-    <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="C62:C67"/>
-    <mergeCell ref="B62:B67"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="C72:C78"/>
-    <mergeCell ref="B72:B78"/>
-    <mergeCell ref="A72:A78"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="B79:B81"/>
-    <mergeCell ref="C79:C81"/>
-    <mergeCell ref="C82:C92"/>
-    <mergeCell ref="B82:B92"/>
-    <mergeCell ref="A82:A92"/>
-    <mergeCell ref="C93:C103"/>
-    <mergeCell ref="B93:B103"/>
-    <mergeCell ref="A93:A103"/>
-    <mergeCell ref="A104:A107"/>
-    <mergeCell ref="B104:B107"/>
-    <mergeCell ref="C104:C107"/>
-    <mergeCell ref="C108:C111"/>
-    <mergeCell ref="B108:B111"/>
-    <mergeCell ref="A108:A111"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="A12:A22"/>
+    <mergeCell ref="B12:B22"/>
+    <mergeCell ref="C12:C22"/>
+    <mergeCell ref="F12:F22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="F7:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>